<commit_message>
Integrated AG Grid for
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -507,7 +507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,11 @@
           <t>Unrealized Profit</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -564,25 +569,28 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>780.01</v>
+        <v>812.52</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>10920.14</v>
+        <v>15437.88</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>4032</v>
+        <v>8153.1</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>6888.14</v>
+        <v>7284.78</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>176.1</v>
       </c>
     </row>
     <row r="3">
@@ -592,7 +600,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>34.1</v>
+        <v>34.66</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>15</v>
@@ -601,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>511.5</v>
+        <v>519.9</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>799.65</v>
@@ -610,7 +618,10 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>-288.15</v>
+        <v>-279.75</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>-35.45</v>
       </c>
     </row>
     <row r="4">
@@ -620,7 +631,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1279.79</v>
+        <v>1285</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -629,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>6398.95</v>
+        <v>6425</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2394</v>
@@ -638,7 +649,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>4004.95</v>
+        <v>4031</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>176.53</v>
       </c>
     </row>
     <row r="5">
@@ -648,7 +662,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>219.4</v>
+        <v>230.47</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>3</v>
@@ -657,7 +671,7 @@
         <v>2750</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>658.2</v>
+        <v>691.41</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>178.26</v>
@@ -666,7 +680,10 @@
         <v>2452.9</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>479.94</v>
+        <v>513.15</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>280.11</v>
       </c>
     </row>
     <row r="6">
@@ -676,7 +693,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>26.47</v>
+        <v>26.17</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>5</v>
@@ -685,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>132.35</v>
+        <v>130.85</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>107.6</v>
@@ -694,7 +711,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>24.75</v>
+        <v>23.25</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>22.86</v>
       </c>
     </row>
     <row r="7">
@@ -704,7 +724,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>144.16</v>
+        <v>147.22</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>12</v>
@@ -713,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>1729.92</v>
+        <v>1766.64</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1680.6</v>
@@ -722,7 +742,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>49.32</v>
+        <v>86.04000000000001</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>4.02</v>
       </c>
     </row>
     <row r="8">
@@ -732,7 +755,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>146.94</v>
+        <v>151.78</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
@@ -741,7 +764,7 @@
         <v>1310</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>146.94</v>
+        <v>151.78</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>155</v>
@@ -750,7 +773,10 @@
         <v>690</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>-8.06</v>
+        <v>-3.22</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>-4.1</v>
       </c>
     </row>
     <row r="9">
@@ -760,7 +786,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>334.78</v>
+        <v>332.04</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>12</v>
@@ -769,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>4017.36</v>
+        <v>3984.48</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>4000.68</v>
@@ -778,7 +804,10 @@
         <v>0</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>16.68</v>
+        <v>-16.2</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>0.82</v>
       </c>
     </row>
     <row r="10">
@@ -788,7 +817,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>552.36</v>
+        <v>552.58</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>5</v>
@@ -797,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2761.8</v>
+        <v>2762.9</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>2785.95</v>
@@ -806,7 +835,10 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>-24.15</v>
+        <v>-23.05</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>-0.46</v>
       </c>
     </row>
     <row r="11">
@@ -816,7 +848,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>177.08</v>
+        <v>187.28</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
@@ -825,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>177.08</v>
+        <v>187.28</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>185</v>
@@ -834,7 +866,103 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>-7.92</v>
+        <v>2.28</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>-3.69</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>RIOT</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>12.25</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>10.55</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>72.04000000000001</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>408.02</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>2040.1</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>1965.1</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>2573.07</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>JBLU</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1209,13 +1337,13 @@
         </is>
       </c>
       <c r="F11" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>155</v>
+        <v>500</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>155</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="12">
@@ -1241,13 +1369,13 @@
         </is>
       </c>
       <c r="F12" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>500</v>
+        <v>155</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>1000</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13">
@@ -1376,6 +1504,198 @@
       </c>
       <c r="H16" s="2" t="n">
         <v>185</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Jonathan R</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>45404</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>RIOT</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>10.51</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>52.55</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Jonathan R</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>45404</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>RIOT</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>10.55</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>10.55</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Joe L</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>45404</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Jonathan R</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>45405</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>JBLU</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Jonathan R</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>45405</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>RIOT</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Jonathan R</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>45405</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>824.22</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>4121.1</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1709,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1438,6 +1758,11 @@
           <t>Unrealized Profit</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1446,25 +1771,28 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>780.01</v>
+        <v>812.52</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>10920.14</v>
+        <v>15437.88</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>4032</v>
+        <v>8153.1</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>6888.14</v>
+        <v>7284.78</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>176.1</v>
       </c>
     </row>
     <row r="3">
@@ -1474,7 +1802,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>34.1</v>
+        <v>34.66</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>15</v>
@@ -1483,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>511.5</v>
+        <v>519.9</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>799.65</v>
@@ -1492,7 +1820,10 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>-288.15</v>
+        <v>-279.75</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>-35.45</v>
       </c>
     </row>
     <row r="4">
@@ -1502,7 +1833,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1279.79</v>
+        <v>1285</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -1511,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>6398.95</v>
+        <v>6425</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2394</v>
@@ -1520,7 +1851,41 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>4004.95</v>
+        <v>4031</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>176.53</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>408.02</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>2040.1</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>1965.1</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>2573.07</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1583,6 +1948,11 @@
           <t>Unrealized Profit</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1591,25 +1961,28 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>780.01</v>
+        <v>812.52</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>10920.14</v>
+        <v>15437.88</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>4032</v>
+        <v>8153.1</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>6888.14</v>
+        <v>7284.78</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>176.1</v>
       </c>
     </row>
     <row r="3">
@@ -1619,7 +1992,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>219.4</v>
+        <v>230.47</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>3</v>
@@ -1628,7 +2001,7 @@
         <v>2750</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>658.2</v>
+        <v>691.41</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>178.26</v>
@@ -1637,7 +2010,10 @@
         <v>2452.9</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>479.94</v>
+        <v>513.15</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>280.11</v>
       </c>
     </row>
     <row r="4">
@@ -1647,7 +2023,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>26.47</v>
+        <v>26.17</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -1656,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>132.35</v>
+        <v>130.85</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>107.6</v>
@@ -1665,7 +2041,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>24.75</v>
+        <v>23.25</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>22.86</v>
       </c>
     </row>
     <row r="5">
@@ -1675,7 +2054,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>144.16</v>
+        <v>147.22</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>12</v>
@@ -1684,7 +2063,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1729.92</v>
+        <v>1766.64</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>1680.6</v>
@@ -1693,7 +2072,72 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>49.32</v>
+        <v>86.04000000000001</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>4.02</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>RIOT</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>12.25</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>10.55</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>72.04000000000001</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>JBLU</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1707,7 +2151,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1756,6 +2200,11 @@
           <t>Unrealized Profit</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1764,7 +2213,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>146.94</v>
+        <v>151.78</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
@@ -1773,7 +2222,7 @@
         <v>1310</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>146.94</v>
+        <v>151.78</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>155</v>
@@ -1782,7 +2231,10 @@
         <v>690</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>-8.06</v>
+        <v>-3.22</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>-4.1</v>
       </c>
     </row>
     <row r="3">
@@ -1792,7 +2244,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>334.78</v>
+        <v>332.04</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>12</v>
@@ -1801,7 +2253,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4017.36</v>
+        <v>3984.48</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>4000.68</v>
@@ -1810,7 +2262,10 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>16.68</v>
+        <v>-16.2</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>0.82</v>
       </c>
     </row>
     <row r="4">
@@ -1820,7 +2275,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>552.36</v>
+        <v>552.58</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -1829,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2761.8</v>
+        <v>2762.9</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2785.95</v>
@@ -1838,7 +2293,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>-24.15</v>
+        <v>-23.05</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>-0.46</v>
       </c>
     </row>
     <row r="5">
@@ -1848,7 +2306,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>177.08</v>
+        <v>187.28</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
@@ -1857,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>177.08</v>
+        <v>187.28</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>185</v>
@@ -1866,7 +2324,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>-7.92</v>
+        <v>2.28</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>-3.69</v>
       </c>
     </row>
   </sheetData>
@@ -1880,7 +2341,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1929,6 +2390,11 @@
           <t>Unrealized Profit</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>